<commit_message>
exporting matrix to csv ans adding functionality to technical documents
</commit_message>
<xml_diff>
--- a/Digital_assets.xlsx
+++ b/Digital_assets.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DIGITAL_ASSETS" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -326,6 +327,30 @@
   </si>
   <si>
     <t xml:space="preserve">247041101-piso-pared-oceano-azul-claro-cd-9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">206191~1.PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246021151-piso-pared-nuevo-tahoe-azul-mt-ft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246021181-piso-pared-nuevo-tahoe-azul-oscuro-mt-ft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246021451-piso-pared-nuevo-tahoe-verde-mt-ft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246021491-piso-pared-nuevo-tahoe-verde-oscuro-mt-ft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247031151-piso-pared-tulum-azul-mt-ft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247031761-piso-pared-tulum-cafe-mt-ft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247041101-piso-pared-oceano-azul-claro-cd-ft.pdf</t>
   </si>
 </sst>
 </file>
@@ -437,12 +462,24 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -527,885 +564,971 @@
   </sheetPr>
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:B109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="130.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="130.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>407971151</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>407971151</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>318004001</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>318004001</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>407918111</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>407918111</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>402911001</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>402911001</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>246021151</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>246021181</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>246021451</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="A56" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>246021491</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B58" s="0" t="s">
+      <c r="A58" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B59" s="0" t="s">
+      <c r="A59" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B60" s="0" t="s">
+      <c r="A60" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B61" s="0" t="s">
+      <c r="A61" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B62" s="0" t="s">
+      <c r="A62" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B63" s="0" t="s">
+      <c r="A63" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B64" s="0" t="s">
+      <c r="A64" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B65" s="0" t="s">
+      <c r="A65" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B66" s="0" t="s">
+      <c r="A66" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B67" s="0" t="s">
+      <c r="A67" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B68" s="0" t="s">
+      <c r="A68" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B69" s="0" t="s">
+      <c r="A69" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B70" s="0" t="s">
+      <c r="A70" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B71" s="0" t="s">
+      <c r="A71" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B72" s="0" t="s">
+      <c r="A72" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B73" s="0" t="s">
+      <c r="A73" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B74" s="0" t="s">
+      <c r="A74" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B75" s="0" t="s">
+      <c r="A75" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B76" s="0" t="s">
+      <c r="A76" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B77" s="0" t="s">
+      <c r="A77" s="1" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B78" s="0" t="s">
+      <c r="A78" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B79" s="0" t="s">
+      <c r="A79" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B80" s="0" t="s">
+      <c r="A80" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B81" s="0" t="s">
+      <c r="A81" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B82" s="0" t="s">
+      <c r="A82" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B83" s="0" t="s">
+      <c r="A83" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B84" s="0" t="s">
+      <c r="A84" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B85" s="0" t="s">
+      <c r="A85" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B86" s="0" t="s">
+      <c r="A86" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B87" s="0" t="s">
+      <c r="A87" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B88" s="0" t="s">
+      <c r="A88" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B89" s="0" t="s">
+      <c r="A89" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B90" s="0" t="s">
+      <c r="A90" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B91" s="0" t="s">
+      <c r="A91" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B92" s="0" t="s">
+      <c r="A92" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B93" s="0" t="s">
+      <c r="A93" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B94" s="0" t="s">
+      <c r="A94" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B95" s="0" t="s">
+      <c r="A95" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B96" s="0" t="s">
+      <c r="A96" s="1" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="n">
+      <c r="A97" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="n">
+      <c r="A98" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="n">
+      <c r="A99" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
+      <c r="A100" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
+      <c r="A101" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="n">
+      <c r="A102" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="n">
+      <c r="A103" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="n">
+      <c r="A104" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="n">
+      <c r="A105" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="n">
+      <c r="A106" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="n">
+      <c r="A107" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="n">
+      <c r="A108" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="n">
+      <c r="A109" s="1" t="n">
         <v>247041101</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="n">
+        <v>246021151</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>246021181</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>246021451</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>246021491</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>247041101</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting to generate a report for the relationship matrixes
</commit_message>
<xml_diff>
--- a/Digital_assets.xlsx
+++ b/Digital_assets.xlsx
@@ -475,11 +475,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,7 +565,7 @@
   <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A1:B8 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
correvting some bugs from the reports generated in the documents matrix generation
</commit_message>
<xml_diff>
--- a/Digital_assets.xlsx
+++ b/Digital_assets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DIGITAL_ASSETS" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t xml:space="preserve">247041101-piso-pared-oceano-azul-claro-cd-9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc123-piso-pared-oceano-azul-claro-cd-7.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc123-piso-pared-oceano-azul-claro-cd-8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc123-piso-pared-oceano-azul-claro-cd-9.png</t>
   </si>
   <si>
     <t xml:space="preserve">206191~1.PDF</t>
@@ -360,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -402,6 +414,14 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -462,7 +482,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,11 +496,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -562,10 +586,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A1:B8 A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B118" activeCellId="0" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1444,6 +1468,33 @@
       <c r="B109" s="1" t="s">
         <v>101</v>
       </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1463,72 +1514,74 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="A1:B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="n">
+      <c r="A1" s="5" t="n">
         <v>246021151</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>246021181</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>246021451</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>246021491</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>247031151</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>247031761</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>247041101</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>246021181</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>246021451</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>246021491</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>247031151</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>247031761</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>247041101</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
-        <v>109</v>
+      <c r="B8" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adadpting digital assets code for videos and prices
</commit_message>
<xml_diff>
--- a/Digital_assets.xlsx
+++ b/Digital_assets.xlsx
@@ -588,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B118" activeCellId="0" sqref="B118"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A1:B1 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>